<commit_message>
29 module staged plus
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -29,10 +29,10 @@
     <t>Университеты</t>
   </si>
   <si>
-    <t>Физика</t>
+    <t>Медицина</t>
   </si>
   <si>
-    <t>Московский Придуманный Институт;Московский Выдуманный Университет;</t>
+    <t>Самарский Медицинский Институт;Московский Государственный Медицинский Университет;Тамбовский Университет Медицины;</t>
   </si>
   <si>
     <t>Математика</t>
@@ -41,10 +41,10 @@
     <t>Казанский Университет Вычислений;</t>
   </si>
   <si>
-    <t>Медицина</t>
+    <t>Физика</t>
   </si>
   <si>
-    <t>Самарский Медицинский Институт;Московский Государственный Медицинский Университет;Тамбовский Университет Медицины;</t>
+    <t>Московский Придуманный Институт;Московский Выдуманный Университет;</t>
   </si>
   <si>
     <t>Лингвистика</t>
@@ -129,13 +129,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>4.539999961853027</v>
+        <v>4.329999923706055</v>
       </c>
       <c r="C2" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="D2" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -163,13 +163,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>4.329999923706055</v>
+        <v>4.539999961853027</v>
       </c>
       <c r="C4" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="D4" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>

</xml_diff>